<commit_message>
new data - total 135283 reviews 1: 21395 2: 7186 3: 11268 4: 21622 5: 73812
</commit_message>
<xml_diff>
--- a/data/places_list.xlsx
+++ b/data/places_list.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -419,10 +419,10 @@
         <v>Review count</v>
       </c>
       <c r="F1" t="str">
+        <v>Link</v>
+      </c>
+      <c r="G1" t="str">
         <v>Scraped</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Link</v>
       </c>
     </row>
     <row r="2">
@@ -441,11 +441,11 @@
       <c r="E2">
         <v>4130</v>
       </c>
-      <c r="F2">
-        <v>903</v>
-      </c>
-      <c r="G2" t="str">
+      <c r="F2" t="str">
         <v>https://www.google.com/maps/place/Cister+Catorce/@36.720286,-4.4176164,17z/data=!4m15!1m8!3m7!1s0xd72f75684ca73cf:0x3ae70cab74ef219b!2sCister+Catorce!8m2!3d36.720286!4d-4.4176164!10e1!16s%2Fg%2F11h2fq_01m!3m5!1s0xd72f75684ca73cf:0x3ae70cab74ef219b!8m2!3d36.720286!4d-4.4176164!16s%2Fg%2F11h2fq_01m?entry=ttu&amp;g_ep=EgoyMDI1MDQxNi4xIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G2">
+        <v>913</v>
       </c>
     </row>
     <row r="3">
@@ -464,11 +464,11 @@
       <c r="E3">
         <v>455505</v>
       </c>
-      <c r="F3">
-        <v>757</v>
-      </c>
-      <c r="G3" t="str">
+      <c r="F3" t="str">
         <v>https://www.google.com/maps/place/Miniera+d'Oro/@45.6331745,7.6440151,9z/data=!3m1!5s0x4786c6dac253c6df:0x61de6d2c3088c186!4m10!1m2!2m1!1sMiniera+d'Oro!3m6!1s0x4786c6c69df35b27:0x3edad3be628f60f1!8m2!3d45.4842841!4d9.2049482!15sCg1NaW5pZXJhIGQnT3JvWg8iDW1pbmllcmEgZCBvcm-SAQtjb2ZmZWVfc2hvcKoBNRABMh4QASIaDLa_tI_x9FAUrgv36p4GL7TD4xTqbDOhUpUyERACIg1taW5pZXJhIGQgb3Jv4AEA!16s%2Fg%2F1pt_zjnl3?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G3">
+        <v>767</v>
       </c>
     </row>
     <row r="4">
@@ -487,11 +487,11 @@
       <c r="E4">
         <v>438804</v>
       </c>
-      <c r="F4">
-        <v>2000</v>
-      </c>
-      <c r="G4" t="str">
+      <c r="F4" t="str">
         <v>https://www.google.com/maps/place/Kolizejs/@41.8905731,12.4897183,17z/data=!4m15!1m8!3m7!1s0x132f61b6fc6433df:0x165f79d5d2332163!2sColosseo,+00184+Roma+RM,+It%C4%81lija!3b1!8m2!3d41.8905691!4d12.4922986!16s%2Fg%2F1q63cjjhd!3m5!1s0x132f61b6532013ad:0x28f1c82e908503c4!8m2!3d41.8902102!4d12.4922309!16zL20vMGQ1cXg?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G4">
+        <v>7057</v>
       </c>
     </row>
     <row r="5">
@@ -510,11 +510,11 @@
       <c r="E5">
         <v>432952</v>
       </c>
-      <c r="F5">
-        <v>2000</v>
-      </c>
-      <c r="G5" t="str">
+      <c r="F5" t="str">
         <v>https://www.google.com/maps/place/Eife%C4%BCa+tornis/@48.8583736,2.291901,17z/data=!3m1!4b1!4m6!3m5!1s0x47e66e2964e34e2d:0x8ddca9ee380ef7e0!8m2!3d48.8583701!4d2.2944813!16zL20vMDJqODE?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G5">
+        <v>7035</v>
       </c>
     </row>
     <row r="6">
@@ -533,11 +533,11 @@
       <c r="E6">
         <v>2153</v>
       </c>
-      <c r="F6">
-        <v>757</v>
-      </c>
-      <c r="G6" t="str">
+      <c r="F6" t="str">
         <v>https://www.google.com/maps/place/Miniera+d'Oro/@45.6331745,7.6440151,9z/data=!3m1!5s0x4786c6dac253c6df:0x61de6d2c3088c186!4m10!1m2!2m1!1sMiniera+d'Oro!3m6!1s0x4786c6c69df35b27:0x3edad3be628f60f1!8m2!3d45.4842841!4d9.2049482!15sCg1NaW5pZXJhIGQnT3JvWg8iDW1pbmllcmEgZCBvcm-SAQtjb2ZmZWVfc2hvcKoBNRABMh4QASIaDLa_tI_x9FAUrgv36p4GL7TD4xTqbDOhUpUyERACIg1taW5pZXJhIGQgb3Jv4AEA!16s%2Fg%2F1pt_zjnl3?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G6">
+        <v>767</v>
       </c>
     </row>
     <row r="7">
@@ -556,11 +556,11 @@
       <c r="E7">
         <v>357</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="str">
+        <v>https://www.google.com/maps/place/KFC/@33.9438983,-118.4128965,17z/data=!3m2!4b1!5s0x80c2b127405f1b81:0x7edf0a3aac8add8e!4m6!3m5!1s0x80c2b178a0d1630b:0x5f5ce4742b568e39!8m2!3d33.9438939!4d-118.4103162!16s%2Fg%2F11c1pkppqf?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G7">
         <v>252</v>
-      </c>
-      <c r="G7" t="str">
-        <v>https://www.google.com/maps/place/KFC/@33.9438983,-118.4128965,17z/data=!3m2!4b1!5s0x80c2b127405f1b81:0x7edf0a3aac8add8e!4m6!3m5!1s0x80c2b178a0d1630b:0x5f5ce4742b568e39!8m2!3d33.9438939!4d-118.4103162!16s%2Fg%2F11c1pkppqf?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
       </c>
     </row>
     <row r="8">
@@ -579,11 +579,11 @@
       <c r="E8">
         <v>3480</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="str">
+        <v>https://www.google.com/maps/place/Park+%26+%E2%80%8B%E2%80%8BControl+Pac+GmbH/@48.6823541,9.20212,17z/data=!3m1!4b1!4m6!3m5!1s0x47a851c9a4bd8067:0x8d2cdd3dc201552f!8m2!3d48.6823506!4d9.2047003!16s%2Fg%2F1hc5pmgz5?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G8">
         <v>85</v>
-      </c>
-      <c r="G8" t="str">
-        <v>https://www.google.com/maps/place/Park+%26+%E2%80%8B%E2%80%8BControl+Pac+GmbH/@48.6823541,9.20212,17z/data=!3m1!4b1!4m6!3m5!1s0x47a851c9a4bd8067:0x8d2cdd3dc201552f!8m2!3d48.6823506!4d9.2047003!16s%2Fg%2F1hc5pmgz5?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
       </c>
     </row>
     <row r="9">
@@ -602,11 +602,11 @@
       <c r="E9">
         <v>1056</v>
       </c>
-      <c r="F9">
-        <v>899</v>
-      </c>
-      <c r="G9" t="str">
+      <c r="F9" t="str">
         <v>https://www.google.com/maps/place/UK+Car+Park+Management+Ltd/@50.8223053,0.2464934,17z/data=!3m2!4b1!5s0x47df71bf03818e03:0x9c5749c35d931543!4m6!3m5!1s0x4875850ae8faa641:0xb7666255b364f340!8m2!3d50.8223019!4d0.2490737!16s%2Fg%2F11c1qdqdpv?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G9">
+        <v>901</v>
       </c>
     </row>
     <row r="10">
@@ -625,11 +625,11 @@
       <c r="E10">
         <v>7335</v>
       </c>
-      <c r="F10">
-        <v>553</v>
-      </c>
-      <c r="G10" t="str">
+      <c r="F10" t="str">
         <v>https://www.google.com/maps/place/Agenskalns+Market/@56.9395162,24.0597702,12z/data=!4m6!3m5!1s0x46eed03da6be4445:0x4d679ef0bbcebb8e!8m2!3d56.9356461!4d24.0715046!16s%2Fg%2F11bzrhmzj3?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G10">
+        <v>558</v>
       </c>
     </row>
     <row r="11">
@@ -648,11 +648,11 @@
       <c r="E11">
         <v>1422</v>
       </c>
-      <c r="F11">
-        <v>541</v>
-      </c>
-      <c r="G11" t="str">
+      <c r="F11" t="str">
         <v>https://www.google.com/maps/place/Caff%C3%A9+Maioli/@43.7673078,11.2501107,17z/data=!3m1!4b1!4m6!3m5!1s0x132a53fffc99a865:0xaed4e7a66c842b66!8m2!3d43.767304!4d11.2526856!16s%2Fg%2F1tfh1x1l?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G11">
+        <v>549</v>
       </c>
     </row>
     <row r="12">
@@ -671,11 +671,11 @@
       <c r="E12">
         <v>1495</v>
       </c>
-      <c r="F12">
-        <v>1324</v>
-      </c>
-      <c r="G12" t="str">
+      <c r="F12" t="str">
         <v>https://www.google.com/maps/place/Planet+Fitness+Club+Support+Center/@42.9497339,-70.8639229,17z/data=!3m1!4b1!4m6!3m5!1s0x89e2bfd44d2d2247:0x385678a0f30bd91d!8m2!3d42.94973!4d-70.861348!16s%2Fg%2F1td5s8jt?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G12">
+        <v>1323</v>
       </c>
     </row>
     <row r="13">
@@ -694,11 +694,11 @@
       <c r="E13">
         <v>1708</v>
       </c>
-      <c r="F13">
-        <v>448</v>
-      </c>
-      <c r="G13" t="str">
+      <c r="F13" t="str">
         <v>https://www.google.com/maps/place/Nonno+Restaurant/@44.8697388,13.839854,17z/data=!3m1!4b1!4m6!3m5!1s0x477cd31df9256a4b:0xa4a8b810b23a4645!8m2!3d44.869735!4d13.8424289!16s%2Fg%2F11c469p9_g?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G13">
+        <v>473</v>
       </c>
     </row>
     <row r="14">
@@ -717,11 +717,11 @@
       <c r="E14">
         <v>1253</v>
       </c>
-      <c r="F14">
-        <v>447</v>
-      </c>
-      <c r="G14" t="str">
+      <c r="F14" t="str">
         <v>https://www.google.com/maps/place/Caff%C3%A8+Arte+Italiana+Srl/@41.9026369,12.4605302,17z/data=!3m2!4b1!5s0x132f605d75dd7c5f:0x26a44557fd65736c!4m6!3m5!1s0x132f610b688773ab:0xad510106189cc4ac!8m2!3d41.9026329!4d12.4631051!16s%2Fg%2F11rss8rj0k?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G14">
+        <v>467</v>
       </c>
     </row>
     <row r="15">
@@ -740,11 +740,11 @@
       <c r="E15">
         <v>1652</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="str">
+        <v>https://www.google.com/maps/place/DPD+Luxembourg+Depot/@49.5080478,6.1053262,17z/data=!3m1!4b1!4m6!3m5!1s0x479537b69599a24d:0x46cd0ba3a79056b3!8m2!3d49.5080443!4d6.1079011!16s%2Fg%2F1tdpqllg?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G15">
         <v>437</v>
-      </c>
-      <c r="G15" t="str">
-        <v>https://www.google.com/maps/place/DPD+Luxembourg+Depot/@49.5080478,6.1053262,17z/data=!3m1!4b1!4m6!3m5!1s0x479537b69599a24d:0x46cd0ba3a79056b3!8m2!3d49.5080443!4d6.1079011!16s%2Fg%2F1tdpqllg?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
       </c>
     </row>
     <row r="16">
@@ -763,11 +763,11 @@
       <c r="E16">
         <v>1557</v>
       </c>
-      <c r="F16">
-        <v>1238</v>
-      </c>
-      <c r="G16" t="str">
+      <c r="F16" t="str">
         <v>https://www.google.com/maps/place/Northwick+Park+Hospital/@51.565073,-0.3733742,13z/data=!4m6!3m5!1s0x487613bcd5331c8b:0x4f4b788138943490!8m2!3d51.5754036!4d-0.3201721!16zL20vMDR0cXBx?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G16">
+        <v>1240</v>
       </c>
     </row>
     <row r="17">
@@ -786,11 +786,11 @@
       <c r="E17">
         <v>2798</v>
       </c>
-      <c r="F17">
-        <v>1392</v>
-      </c>
-      <c r="G17" t="str">
+      <c r="F17" t="str">
         <v>https://www.google.com/maps/place/B%26Q+Yeading/@51.5521527,-0.4469848,13z/data=!4m6!3m5!1s0x48766d519713acb3:0x94727317752f3e51!8m2!3d51.5226482!4d-0.387927!16s%2Fg%2F1tngpsl_?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G17">
+        <v>1397</v>
       </c>
     </row>
     <row r="18">
@@ -809,11 +809,11 @@
       <c r="E18">
         <v>1113</v>
       </c>
-      <c r="F18">
-        <v>563</v>
-      </c>
-      <c r="G18" t="str">
+      <c r="F18" t="str">
         <v>https://www.google.com/maps/place/Asda+Govan+Superstore/@55.8642165,-4.3125924,14z/data=!3m1!5s0x4888460f6c7a527f:0xf4e26066f8da551b!4m6!3m5!1s0x4888460ee28add97:0xc31a86abcbf04400!8m2!3d55.852668!4d-4.3225573!16s%2Fg%2F1td250f6?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G18">
+        <v>564</v>
       </c>
     </row>
     <row r="19">
@@ -832,11 +832,11 @@
       <c r="E19">
         <v>36121</v>
       </c>
-      <c r="F19">
-        <v>2000</v>
-      </c>
-      <c r="G19" t="str">
+      <c r="F19" t="str">
         <v>https://www.google.com/maps/place/London+Stansted+Airport/@51.8863747,-0.0635548,11z/data=!4m10!1m2!2m1!1sairport!3m6!1s0x487604b8a52a1bb7:0x30a4d0976b352648!8m2!3d51.8863747!4d0.2413158!15sCgdhaXJwb3J0WgkiB2FpcnBvcnSSARVpbnRlcm5hdGlvbmFsX2FpcnBvcnSqATwQASoLIgdhaXJwb3J0KAAyHhABIhoyqn08Egw-gILFZbHpRXxdNsV4vgiTu0DuuTILEAIiB2FpcnBvcnTgAQA!16zL20vMGhjc2g?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G19">
+        <v>6678</v>
       </c>
     </row>
     <row r="20">
@@ -855,11 +855,11 @@
       <c r="E20">
         <v>10340</v>
       </c>
-      <c r="F20">
-        <v>1579</v>
-      </c>
-      <c r="G20" t="str">
+      <c r="F20" t="str">
         <v>https://www.google.com/maps/place/Giovan+Battista+Pastine+International+Airport/@41.049465,-1.2763489,5z/data=!4m10!1m2!2m1!1sairport+italy!3m6!1s0x132588b6389de903:0xedb6061d8fc5510d!8m2!3d41.7992296!4d12.5931741!15sCg1haXJwb3J0IGl0YWx5kgEVaW50ZXJuYXRpb25hbF9haXJwb3J0qgFCEAEqCyIHYWlycG9ydCgAMh4QASIa2vwLF099pRKRe9ZHW5K3MDXHcBi9DVp5DtgyERACIg1haXJwb3J0IGl0YWx54AEA!16zL20vMDMzXzUy?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G20">
+        <v>1583</v>
       </c>
     </row>
     <row r="21">
@@ -878,11 +878,11 @@
       <c r="E21">
         <v>34850</v>
       </c>
-      <c r="F21">
-        <v>2000</v>
-      </c>
-      <c r="G21" t="str">
+      <c r="F21" t="str">
         <v>https://www.google.com/maps/place/Paris+Orly+Airport/@48.8451848,2.1953304,11z/data=!4m9!1m2!2m1!1sairport+italy!3m5!1s0x47e675b1fa6a3b1d:0x9d78ded743db8422!8m2!3d48.7299182!4d2.3732304!16zL20vMDFsNTI1?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G21">
+        <v>2816</v>
       </c>
     </row>
     <row r="22">
@@ -901,11 +901,11 @@
       <c r="E22">
         <v>6259</v>
       </c>
-      <c r="F22">
-        <v>410</v>
-      </c>
-      <c r="G22" t="str">
+      <c r="F22" t="str">
         <v>https://www.google.com/maps/place/Cit%C3%A9+des+Sciences+et+de+l'Industrie/@48.8667009,2.2528369,13z/data=!4m9!1m2!2m1!1sairport+italy!3m5!1s0x47e66c32df92aa0f:0x52d157d86ddecf27!8m2!3d48.8955948!4d2.3878996!16zL20vMDliaHY0?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G22">
+        <v>412</v>
       </c>
     </row>
     <row r="23">
@@ -924,11 +924,11 @@
       <c r="E23">
         <v>1923</v>
       </c>
-      <c r="F23">
-        <v>537</v>
-      </c>
-      <c r="G23" t="str">
+      <c r="F23" t="str">
         <v>https://www.google.com/maps/place/ibis+budget+Zurich+City+West/@47.3922115,8.5197683,14z/data=!4m6!3m5!1s0x47900a4748aa2f71:0x4e9e32bac8607920!8m2!3d47.3889874!4d8.5162188!16s%2Fg%2F1td41dn0?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G23">
+        <v>542</v>
       </c>
     </row>
     <row r="24">
@@ -947,11 +947,11 @@
       <c r="E24">
         <v>6353</v>
       </c>
-      <c r="F24">
-        <v>2000</v>
-      </c>
-      <c r="G24" t="str">
+      <c r="F24" t="str">
         <v>https://www.google.com/maps/place/The+Roosevelt+Hotel/@40.7546645,-73.9798117,17z/data=!3m1!4b1!4m6!3m5!1s0x89c258fe06a22399:0x206b4253a07248e8!8m2!3d40.7546645!4d-73.9772368!16s%2Fm%2F0gx16n2?entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G24">
+        <v>2964</v>
       </c>
     </row>
     <row r="25">
@@ -970,11 +970,11 @@
       <c r="E25">
         <v>6984</v>
       </c>
-      <c r="F25">
-        <v>648</v>
-      </c>
-      <c r="G25" t="str">
+      <c r="F25" t="str">
         <v>https://www.google.com/maps/place/Hotel+Flamingo+All+Inclusive/@21.1177855,-86.7594424,17z/data=!3m1!4b1!4m6!3m5!1s0x8f4c2b0d61aaaaab:0x972182d84386ea65!8m2!3d21.1177805!4d-86.7568675!16s%2Fg%2F1tcyyh0j?hl=en&amp;entry=ttu&amp;g_ep=EgoyMDI1MDQyMy4wIKXMDSoJLDEwMjExNjQwSAFQAw%3D%3D</v>
+      </c>
+      <c r="G25">
+        <v>650</v>
       </c>
     </row>
     <row r="26">
@@ -993,11 +993,11 @@
       <c r="E26">
         <v>106896</v>
       </c>
-      <c r="F26">
-        <v>220</v>
-      </c>
-      <c r="G26" t="str">
+      <c r="F26" t="str">
         <v>https://www.google.com/maps/place/Statue+of+Liberty/@40.6892534,-74.0470807,17z/data=!3m1!4b1!4m6!3m5!1s0x89c25090129c363d:0x40c6a5770d25022b!8m2!3d40.6892494!4d-74.0445004!16zL20vMDcycDg?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G26">
+        <v>7055</v>
       </c>
     </row>
     <row r="27">
@@ -1016,11 +1016,11 @@
       <c r="E27">
         <v>256620</v>
       </c>
-      <c r="F27">
-        <v>110</v>
-      </c>
-      <c r="G27" t="str">
+      <c r="F27" t="str">
         <v>https://www.google.com/maps/place/Walt+Disney+World%C2%AE+Resort/@28.3771903,-81.5756056,17z/data=!3m1!4b1!4m6!3m5!1s0x88dd7ee634caa5f7:0xa71e391fd01cf1a0!8m2!3d28.3771857!4d-81.57074!16zL20vMDliMWs?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G27">
+        <v>6802</v>
       </c>
     </row>
     <row r="28">
@@ -1039,11 +1039,11 @@
       <c r="E28">
         <v>112827</v>
       </c>
-      <c r="F28">
-        <v>2000</v>
-      </c>
-      <c r="G28" t="str">
+      <c r="F28" t="str">
         <v>https://www.google.com/maps/place/Tower+of+London/@51.5081157,-0.0785296,17z/data=!3m1!4b1!4m6!3m5!1s0x48760349331f38dd:0xa8bf49dde1d56467!8m2!3d51.5081124!4d-0.0759493!16zL20vMDducW4?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G28">
+        <v>7096</v>
       </c>
     </row>
     <row r="29">
@@ -1062,11 +1062,11 @@
       <c r="E29">
         <v>55079</v>
       </c>
-      <c r="F29">
-        <v>2000</v>
-      </c>
-      <c r="G29" t="str">
+      <c r="F29" t="str">
         <v>https://www.google.com/maps/place/The+National+Gallery/@51.5089323,-0.1308793,17z/data=!3m1!4b1!4m6!3m5!1s0x487604ce176ac979:0x42af85654e23a0b4!8m2!3d51.508929!4d-0.128299!16zL20vMHA4OGo?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G29">
+        <v>5272</v>
       </c>
     </row>
     <row r="30">
@@ -1085,11 +1085,11 @@
       <c r="E30">
         <v>345010</v>
       </c>
-      <c r="F30">
-        <v>2000</v>
-      </c>
-      <c r="G30" t="str">
+      <c r="F30" t="str">
         <v>https://www.google.com/maps/place/Louvre+Museum/@48.8606146,2.3350637,17z/data=!3m2!4b1!5s0x47f112d46c2f6eef:0xfb8a933f53aec2c6!4m6!3m5!1s0x47e671d877937b0f:0xb975fcfa192f84d4!8m2!3d48.8606111!4d2.337644!16zL20vMDRnZHI?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G30">
+        <v>2837</v>
       </c>
     </row>
     <row r="31">
@@ -1108,11 +1108,11 @@
       <c r="E31">
         <v>57532</v>
       </c>
-      <c r="F31">
-        <v>200</v>
-      </c>
-      <c r="G31" t="str">
+      <c r="F31" t="str">
         <v>https://www.google.com/maps/place/Hollywood+Walk+of+Fame/@34.1016059,-118.3390966,16z/data=!4m10!1m2!2m1!1sHollywood+Walk+of+Fame!3m6!1s0x80c2bf3b59bb205f:0x85775770084cf53e!8m2!3d34.1016059!4d-118.3295694!15sChZIb2xseXdvb2QgV2FsayBvZiBGYW1lWhgiFmhvbGx5d29vZCB3YWxrIG9mIGZhbWWSARNoaXN0b3JpY2FsX2xhbmRtYXJrqgFQEAEqECIMd2FsayBvZiBmYW1lKAAyHhABIhraBCr57dKNSVcy5SMiQOXoGil6R6RaXlfvajIaEAIiFmhvbGx5d29vZCB3YWxrIG9mIGZhbWXgAQA!16s%2Fg%2F122d85wl?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G31">
+        <v>5039</v>
       </c>
     </row>
     <row r="32">
@@ -1131,11 +1131,11 @@
       <c r="E32">
         <v>79392</v>
       </c>
-      <c r="F32">
-        <v>2000</v>
-      </c>
-      <c r="G32" t="str">
+      <c r="F32" t="str">
         <v>https://www.google.com/maps/place/CN+Tower/@43.6425701,-79.3896371,17z/data=!3m2!4b1!5s0x882b34d819a55ff7:0xad7cf7bcaf4e239b!4m6!3m5!1s0x882b34d68bf33a9b:0x15edd8c4de1c7581!8m2!3d43.6425662!4d-79.3870568!16zL20vMDF0d3M?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G32">
+        <v>5331</v>
       </c>
     </row>
     <row r="33">
@@ -1154,11 +1154,11 @@
       <c r="E33">
         <v>12184</v>
       </c>
-      <c r="F33">
-        <v>2004</v>
-      </c>
-      <c r="G33" t="str">
+      <c r="F33" t="str">
         <v>https://www.google.com/maps/place/Fairmont+Royal+York/@43.6460342,-79.3839683,17z/data=!4m9!3m8!1s0x882b34d3152a8e61:0x154fe230e73270f!5m2!4m1!1i2!8m2!3d43.6460303!4d-79.381388!16zL20vMDRsbl9k?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G33">
+        <v>5042</v>
       </c>
     </row>
     <row r="34">
@@ -1177,11 +1177,11 @@
       <c r="E34">
         <v>61393</v>
       </c>
-      <c r="F34">
-        <v>2000</v>
-      </c>
-      <c r="G34" t="str">
+      <c r="F34" t="str">
         <v>https://www.google.com/maps/place/Heathrow+Airport/@51.4710479,-0.4866857,14z/data=!3m2!4b1!5s0x487673b8f6eefc23:0xf291f2881d9258d5!4m6!3m5!1s0x48767234cdc56de9:0x8fe7535543f64167!8m2!3d51.4679914!4d-0.455051!16zL20vMDNqbjQ?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G34">
+        <v>5024</v>
       </c>
     </row>
     <row r="35">
@@ -1200,11 +1200,11 @@
       <c r="E35">
         <v>77317</v>
       </c>
-      <c r="F35">
-        <v>2000</v>
-      </c>
-      <c r="G35" t="str">
+      <c r="F35" t="str">
         <v>https://www.google.com/maps/place/The+O2/@51.502979,-0.0062934,16z/data=!3m2!4b1!5s0x47d8a81ce55fb6cf:0xd17024fbebc06a05!4m6!3m5!1s0x47d8a81c5507b387:0x981ded0cf3b9dadf!8m2!3d51.503038!4d0.0031543!16s%2Fm%2F047t9qn?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G35">
+        <v>5251</v>
       </c>
     </row>
     <row r="36">
@@ -1223,11 +1223,11 @@
       <c r="E36">
         <v>16113</v>
       </c>
-      <c r="F36">
-        <v>2000</v>
-      </c>
-      <c r="G36" t="str">
+      <c r="F36" t="str">
         <v>https://www.google.com/maps/place/Sydney+Airport/@-33.9354304,151.1618103,15z/data=!3m1!4b1!4m6!3m5!1s0x6b12b0f11b3383db:0xafdf355d5a4b6577!8m2!3d-33.9500314!4d151.1816944!16zL20vMDFuZmwx?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G36">
+        <v>3431</v>
       </c>
     </row>
     <row r="37">
@@ -1246,8 +1246,11 @@
       <c r="E37">
         <v>5011</v>
       </c>
-      <c r="G37" t="str">
+      <c r="F37" t="str">
         <v>www.google.com/maps/place/Bondi+Beach/@-33.8923627,151.2754982,17z/data=!3m1!4b1!4m6!3m5!1s0x6b12ad9c447281c7:0x20c31809c62de978!8m2!3d-33.8914755!4d151.2766845!16zL20vMDIwNzcy?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G37">
+        <v>2138</v>
       </c>
     </row>
     <row r="38">
@@ -1266,11 +1269,11 @@
       <c r="E38">
         <v>665</v>
       </c>
-      <c r="F38">
-        <v>468</v>
-      </c>
-      <c r="G38" t="str">
+      <c r="F38" t="str">
         <v>https://www.google.com/maps/place/Crowne+Plaza+Sydney+Darling+Harbour+by+IHG/@-33.8740127,151.2019918,17z/data=!3m1!5s0x6b12ae3bf804e923:0x963a1e7f49e64f6e!4m9!3m8!1s0x6b12afc17624f033:0x40eba3a4120653a2!5m2!4m1!1i2!8m2!3d-33.8740172!4d151.2045721!16s%2Fg%2F11h585fkyy?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G38">
+        <v>469</v>
       </c>
     </row>
     <row r="39">
@@ -1289,11 +1292,11 @@
       <c r="E39">
         <v>24600</v>
       </c>
-      <c r="F39">
-        <v>2000</v>
-      </c>
-      <c r="G39" t="str">
+      <c r="F39" t="str">
         <v>https://www.google.com/maps/place/Melbourne+Central/@-37.8102318,144.9601849,17z/data=!3m2!4b1!5s0x6ad642caee3d1e1d:0xe2c955d3e9fc08a0!4m6!3m5!1s0x6ad642cae530b1c9:0x59444c336aced016!8m2!3d-37.8102361!4d144.9627652!16zL20vMGNqc21t?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G39">
+        <v>5184</v>
       </c>
     </row>
     <row r="40">
@@ -1312,11 +1315,11 @@
       <c r="E40">
         <v>41670</v>
       </c>
-      <c r="F40">
-        <v>2000</v>
-      </c>
-      <c r="G40" t="str">
+      <c r="F40" t="str">
         <v>https://www.google.com/maps/place/Toronto+Pearson+International+Airport/@43.6821892,-79.6320082,15z/data=!3m1!4b1!4m6!3m5!1s0x882b394ac02dd491:0xb41d5de9c4030ec5!8m2!3d43.6798345!4d-79.6283834!16zL20vMDZrOWw3?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G40">
+        <v>5018</v>
       </c>
     </row>
     <row r="41">
@@ -1335,11 +1338,11 @@
       <c r="E41">
         <v>53459</v>
       </c>
-      <c r="F41">
-        <v>2000</v>
-      </c>
-      <c r="G41" t="str">
+      <c r="F41" t="str">
         <v>https://www.google.com/maps/place/West+Edmonton+Mall/@53.5230503,-113.6253218,17z/data=!3m2!4b1!5s0x53a0205978313b13:0xff95595efd0ba9bb!4m6!3m5!1s0x53a020573a8614db:0x8546a29e09b26fcb!8m2!3d53.5230471!4d-113.6227415!16zL20vMDFwZndw?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G41">
+        <v>5291</v>
       </c>
     </row>
     <row r="42">
@@ -1358,11 +1361,11 @@
       <c r="E42">
         <v>34199</v>
       </c>
-      <c r="F42">
-        <v>2000</v>
-      </c>
-      <c r="G42" t="str">
+      <c r="F42" t="str">
         <v>https://www.google.com/maps/place/Dublin+Airport/@53.4266883,-6.2498372,16z/data=!3m1!4b1!4m6!3m5!1s0x486711be6993192f:0x55121bb5b725f355!8m2!3d53.425632!4d-6.2573755!16zL20vMDFxeWt0?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G42">
+        <v>5020</v>
       </c>
     </row>
     <row r="43">
@@ -1381,11 +1384,11 @@
       <c r="E43">
         <v>21991</v>
       </c>
-      <c r="F43">
-        <v>2000</v>
-      </c>
-      <c r="G43" t="str">
+      <c r="F43" t="str">
         <v>https://www.google.com/maps/place/Guinness+Storehouse/@53.341812,-6.2892958,17z/data=!3m1!4b1!4m6!3m5!1s0x48670e8440c5056b:0xb31933927505e7a2!8m2!3d53.3418088!4d-6.2867155!16s%2Fm%2F02p9xg3?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G43">
+        <v>5193</v>
       </c>
     </row>
     <row r="44">
@@ -1404,17 +1407,86 @@
       <c r="E44">
         <v>1259</v>
       </c>
-      <c r="F44">
-        <v>420</v>
-      </c>
-      <c r="G44" t="str">
+      <c r="F44" t="str">
         <v>https://www.google.com/maps/place/Trinity+College+Library/@53.3439553,-6.2590186,18z/data=!4m10!1m2!2m1!1sTrinity+College+Library+!3m6!1s0x48670e9b4704d255:0xd45b0857d96ad06c!8m2!3d53.3439553!4d-6.2566368!15sChdUcmluaXR5IENvbGxlZ2UgTGlicmFyeSIDiAEBWhkiF3RyaW5pdHkgY29sbGVnZSBsaWJyYXJ5kgEHbGlicmFyeaoBYwoNL2cvMTFjc3E3dDdjOQoJL20vMDExeHkxCggvbS8wNGg4aBABMh4QASIa_YnrCOfWaTzwen8PKIKrWLnvO8aKCVsPdCAyGxACIhd0cmluaXR5IGNvbGxlZ2UgbGlicmFyeeABAA!16s%2Fg%2F11b7g1y8vh?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G44">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Budget Inn</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Austin</v>
+      </c>
+      <c r="C45" t="str">
+        <v>USA</v>
+      </c>
+      <c r="D45">
+        <v>2.6</v>
+      </c>
+      <c r="E45">
+        <v>968</v>
+      </c>
+      <c r="F45" t="str">
+        <v>https://www.google.com/maps/place/Budget+Inn/@30.3577993,-97.6961731,14.08z/data=!4m24!1m13!3m12!1s0x8644c97b01a97cd5:0x75ae0ed3206a869c!2sBudget+Inn!5m3!1s2025-06-22!4m1!1i2!8m2!3d30.3566069!4d-97.690068!9m1!1b1!16s%2Fg%2F1tfshswb!3m9!1s0x8644c97b01a97cd5:0x75ae0ed3206a869c!5m3!1s2025-06-22!4m1!1i2!8m2!3d30.3566069!4d-97.690068!16s%2Fg%2F1tfshswb?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G45">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>China Mall Jhb</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Johannesburg</v>
+      </c>
+      <c r="C46" t="str">
+        <v>South Africa</v>
+      </c>
+      <c r="D46">
+        <v>3.9</v>
+      </c>
+      <c r="E46">
+        <v>25884</v>
+      </c>
+      <c r="F46" t="str">
+        <v>https://www.google.com/maps/place/China+Mall+Jhb/@-24.1066306,28.8608465,5.92z/data=!4m16!1m9!3m8!1s0x1e9509f27788b31d:0xd8cdc5c977fa8a06!2sChina+Mall+Jhb!8m2!3d-26.2140349!4d28.0022176!9m1!1b1!16s%2Fg%2F11jxxf3y2k!3m5!1s0x1e9509f27788b31d:0xd8cdc5c977fa8a06!8m2!3d-26.2140349!4d28.0022176!16s%2Fg%2F11jxxf3y2k?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G46">
+        <v>5059</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Copenhagen Downtown Hostel</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Copenhagen</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Denmark</v>
+      </c>
+      <c r="D47">
+        <v>3.9</v>
+      </c>
+      <c r="E47">
+        <v>3445</v>
+      </c>
+      <c r="F47" t="str">
+        <v>https://www.google.com/maps/place/Copenhagen+Downtown+Hostel/@55.7130528,12.6202962,10.71z/data=!4m10!3m9!1s0x46525313d7b872d7:0x67a1c9c1ceb669f3!5m3!1s2025-06-22!4m1!1i2!8m2!3d55.6759836!4d12.5743854!16s%2Fg%2F1tfkd5wr?entry=ttu&amp;g_ep=EgoyMDI1MDYxNi4wIKXMDSoASAFQAw%3D%3D</v>
+      </c>
+      <c r="G47">
+        <v>1316</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G44"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>